<commit_message>
There's a bug with removing records from original dataset on the saving screen
</commit_message>
<xml_diff>
--- a/Files/lpsC.xlsx
+++ b/Files/lpsC.xlsx
@@ -58,88 +58,88 @@
     <t>G</t>
   </si>
   <si>
+    <t>FDL</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>FDR</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>BUR</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>BUL</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>BDR</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>BDL</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>LUB</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
     <t>FUL</t>
   </si>
   <si>
     <t>Q</t>
   </si>
   <si>
-    <t>FDL</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>FDR</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>BUR</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>BUL</t>
-  </si>
-  <si>
-    <t>M</t>
+    <t>LDB</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>LUF</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>LDF</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>RDF</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>RUB</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
   <si>
     <t>RDB</t>
   </si>
   <si>
     <t>Z</t>
-  </si>
-  <si>
-    <t>BDR</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>BDL</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>LUB</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>LDB</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>LUF</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>LDF</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>RFD</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>RUB</t>
-  </si>
-  <si>
-    <t>W</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -577,7 +577,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -601,7 +601,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -633,7 +633,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
There's a bug with removing records from original dataset on the saving screen. Probably fixed
</commit_message>
<xml_diff>
--- a/Files/lpsC.xlsx
+++ b/Files/lpsC.xlsx
@@ -58,88 +58,88 @@
     <t>G</t>
   </si>
   <si>
+    <t>FDL</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>FDR</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>BUR</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>BUL</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>BDR</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>BDL</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>LUB</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
     <t>FUL</t>
   </si>
   <si>
     <t>Q</t>
   </si>
   <si>
-    <t>FDL</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
-    <t>FDR</t>
-  </si>
-  <si>
-    <t>K</t>
-  </si>
-  <si>
-    <t>BUR</t>
-  </si>
-  <si>
-    <t>L</t>
-  </si>
-  <si>
-    <t>BUL</t>
-  </si>
-  <si>
-    <t>M</t>
+    <t>LDB</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>LUF</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>LDF</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>RDF</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>RUB</t>
+  </si>
+  <si>
+    <t>W</t>
   </si>
   <si>
     <t>RDB</t>
   </si>
   <si>
     <t>Z</t>
-  </si>
-  <si>
-    <t>BDR</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>BDL</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>LUB</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>LDB</t>
-  </si>
-  <si>
-    <t>R</t>
-  </si>
-  <si>
-    <t>LUF</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>LDF</t>
-  </si>
-  <si>
-    <t>T</t>
-  </si>
-  <si>
-    <t>RFD</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>RUB</t>
-  </si>
-  <si>
-    <t>W</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -577,7 +577,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -601,7 +601,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -633,7 +633,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>